<commit_message>
SMASUNG  7.0.0 and Huwawei are OK
</commit_message>
<xml_diff>
--- a/table_device_package.xlsx
+++ b/table_device_package.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T0173711\appkillermanager_exemple\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\StudioProjects\AppKillerManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>DEVICES</t>
   </si>
@@ -272,6 +272,9 @@
       </rPr>
       <t>;  protect activity</t>
     </r>
+  </si>
+  <si>
+    <t>com.samsung.android.sm.ui.battery.AppSleepListActivity</t>
   </si>
 </sst>
 </file>
@@ -657,26 +660,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="149.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="112.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="69.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="91.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="75.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="62.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="149.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="112.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="91.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="75.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -752,7 +755,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="105">
+    <row r="3" spans="1:15" ht="100.8">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -811,7 +814,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="45">
+    <row r="5" spans="1:15" ht="43.2">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -828,7 +831,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="60">
+    <row r="6" spans="1:15" ht="57.6">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -868,7 +871,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="30">
+    <row r="8" spans="1:15" ht="28.8">
       <c r="B8" s="5" t="s">
         <v>64</v>
       </c>
@@ -888,6 +891,9 @@
     <row r="9" spans="1:15">
       <c r="E9" t="s">
         <v>55</v>
+      </c>
+      <c r="H9" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:15">

</xml_diff>

<commit_message>
add some info as commentary add Xiaomi Support
</commit_message>
<xml_diff>
--- a/table_device_package.xlsx
+++ b/table_device_package.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\StudioProjects\AppKillerManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T0173711\AndroidStudioProjects\AppKillerManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>DEVICES</t>
   </si>
@@ -275,13 +275,115 @@
   </si>
   <si>
     <t>com.samsung.android.sm.ui.battery.AppSleepListActivity</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">private static final </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">String </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF9876AA"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">MIUI_ACTION </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"miui.intent.action.APP_PERM_EDITOR"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">private static final </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">String </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF9876AA"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">MIUI_EXTRA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"extra_pkgname"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,6 +432,25 @@
       <name val="Lucida Sans Typewriter"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC7832"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF9876AA"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -357,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -376,6 +497,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -660,26 +787,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="75.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="149.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="112.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="62.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="69.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="91.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="75.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="62.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="149.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="112.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="91.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -755,7 +882,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="100.8">
+    <row r="3" spans="1:15" ht="105">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -814,7 +941,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="43.2">
+    <row r="5" spans="1:15" ht="45">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -831,7 +958,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="57.6">
+    <row r="6" spans="1:15" ht="60">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -871,10 +998,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="28.8">
+    <row r="8" spans="1:15" ht="30">
       <c r="B8" s="5" t="s">
         <v>64</v>
       </c>
+      <c r="C8" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="E8" t="s">
         <v>54</v>
       </c>
@@ -889,6 +1019,9 @@
       </c>
     </row>
     <row r="9" spans="1:15">
+      <c r="C9" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="E9" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
tow amazing lib to help
</commit_message>
<xml_diff>
--- a/table_device_package.xlsx
+++ b/table_device_package.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T0173711\AndroidStudioProjects\AppKillerManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\StudioProjects\AppKillerManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>DEVICES</t>
   </si>
@@ -376,6 +376,29 @@
         <family val="3"/>
       </rPr>
       <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"com.huawei.systemmanager"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF032F62"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"com.huawei.systemmanager.optimize.bootstart.BootStartActivity"</t>
     </r>
   </si>
 </sst>
@@ -383,7 +406,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,6 +472,18 @@
       <sz val="10"/>
       <color rgb="FF9876AA"/>
       <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF032F62"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF24292E"/>
+      <name val="Consolas"/>
       <family val="3"/>
     </font>
   </fonts>
@@ -478,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -505,6 +540,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,28 +821,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="149.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="112.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="69.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="91.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="75.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="62.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="149.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="112.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="91.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="75.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -882,7 +918,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="105">
+    <row r="3" spans="1:15" ht="100.8">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -941,7 +977,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="45">
+    <row r="5" spans="1:15" ht="43.2">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -958,7 +994,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="60">
+    <row r="6" spans="1:15" ht="57.6">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -998,7 +1034,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="30">
+    <row r="8" spans="1:15" ht="28.8">
       <c r="B8" s="5" t="s">
         <v>64</v>
       </c>
@@ -1037,6 +1073,11 @@
     <row r="11" spans="1:15">
       <c r="E11" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="E13" s="10" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve readMe, fix maven package name
</commit_message>
<xml_diff>
--- a/table_device_package.xlsx
+++ b/table_device_package.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\StudioProjects\AppKillerManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T0173711\AndroidStudioProjects\AppKillerManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -227,53 +227,6 @@
        "com.coloros.powermanager.fuelgaue.PowerConsumptionActivity"</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF9876AA"/>
-        <rFont val="Lucida Sans Typewriter"/>
-        <family val="3"/>
-      </rPr>
-      <t>work + intent</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="Lucida Sans Typewriter"/>
-        <family val="3"/>
-      </rPr>
-      <t>.setAction(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="Lucida Sans Typewriter"/>
-        <family val="3"/>
-      </rPr>
-      <t>"huawei.intent.action.HSM_PROTECTED_APPS"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="Lucida Sans Typewriter"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.3"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="Lucida Sans Typewriter"/>
-        <family val="3"/>
-      </rPr>
-      <t>;  protect activity</t>
-    </r>
-  </si>
-  <si>
     <t>com.samsung.android.sm.ui.battery.AppSleepListActivity</t>
   </si>
   <si>
@@ -399,6 +352,53 @@
         <family val="3"/>
       </rPr>
       <t>"com.huawei.systemmanager.optimize.bootstart.BootStartActivity"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF9876AA"/>
+        <rFont val="Lucida Sans Typewriter"/>
+        <family val="3"/>
+      </rPr>
+      <t>work : intent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Lucida Sans Typewriter"/>
+        <family val="3"/>
+      </rPr>
+      <t>.setAction(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Lucida Sans Typewriter"/>
+        <family val="3"/>
+      </rPr>
+      <t>"huawei.intent.action.HSM_PROTECTED_APPS"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Lucida Sans Typewriter"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.3"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Lucida Sans Typewriter"/>
+        <family val="3"/>
+      </rPr>
+      <t>;  protect activity</t>
     </r>
   </si>
 </sst>
@@ -823,26 +823,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="75.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="149.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="112.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="62.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="69.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="91.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="75.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="62.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="149.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="112.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="91.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -918,7 +918,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="100.8">
+    <row r="3" spans="1:15" ht="105">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -977,7 +977,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="43.2">
+    <row r="5" spans="1:15" ht="45">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -994,7 +994,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="57.6">
+    <row r="6" spans="1:15" ht="60">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>59</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>26</v>
@@ -1034,12 +1034,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="28.8">
+    <row r="8" spans="1:15" ht="30">
       <c r="B8" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" t="s">
         <v>54</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="9" spans="1:15">
       <c r="C9" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
         <v>55</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1077,7 +1077,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="E13" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refractor and add meizu
</commit_message>
<xml_diff>
--- a/table_device_package.xlsx
+++ b/table_device_package.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T0173711\AndroidStudioProjects\AppKillerManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\StudioProjects\AppKillerManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>DEVICES</t>
   </si>
@@ -400,6 +400,18 @@
       </rPr>
       <t>;  protect activity</t>
     </r>
+  </si>
+  <si>
+    <t>"com.meizu.safe.cleaner.RubbishCleanMainActivity"</t>
+  </si>
+  <si>
+    <t>"com.meizu.safe.powerui.AppPowerManagerActivity"</t>
+  </si>
+  <si>
+    <t>"com.meizu.safe.ramcleaner.RAMCleanerWhiteList" 3,7</t>
+  </si>
+  <si>
+    <t>com.meizu.safe.permission.NotificationActivity 3,7</t>
   </si>
 </sst>
 </file>
@@ -823,26 +835,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="149.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="112.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="69.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="91.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="75.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="62.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="149.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="112.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="91.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="75.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -918,7 +930,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="105">
+    <row r="3" spans="1:15" ht="100.8">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -977,7 +989,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="45">
+    <row r="5" spans="1:15" ht="43.2">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -994,7 +1006,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="60">
+    <row r="6" spans="1:15" ht="57.6">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1033,8 +1045,11 @@
       <c r="H7" t="s">
         <v>52</v>
       </c>
+      <c r="I7" s="10" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" ht="30">
+    <row r="8" spans="1:15" ht="28.8">
       <c r="B8" s="5" t="s">
         <v>64</v>
       </c>
@@ -1049,6 +1064,9 @@
       </c>
       <c r="H8" t="s">
         <v>53</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="N8" t="s">
         <v>51</v>
@@ -1064,10 +1082,16 @@
       <c r="H9" t="s">
         <v>65</v>
       </c>
+      <c r="I9" s="10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="E10" t="s">
         <v>57</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:15">

</xml_diff>

<commit_message>
Add letv, add readme informations
</commit_message>
<xml_diff>
--- a/table_device_package.xlsx
+++ b/table_device_package.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\StudioProjects\AppKillerManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T0173711\AndroidStudioProjects\AppKillerManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>DEVICES</t>
   </si>
@@ -509,6 +509,74 @@
         <rFont val="Inherit"/>
       </rPr>
       <t>))</t>
+    </r>
+  </si>
+  <si>
+    <t>ONEPLUS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>".ChainLaunchAppListActivity"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">autostart : new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>ComponentName(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"com.oneplus.security"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">"com.oneplus.security.chainlaunch.view" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>+new ComponentName("com.oneplus.security", "com.oneplus.security.chainlaunch.view" +
+                ".ChainLaunchAppListActivity"</t>
     </r>
   </si>
 </sst>
@@ -656,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -692,6 +760,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -973,282 +1047,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="75.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="149.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="112.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="62.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="69.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="91.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="75.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="62.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="94.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="149.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="112.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="72.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="91.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:16">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>40</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>42</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>43</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="100.8">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:16" ht="364.5">
+      <c r="B3" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="L3" t="s">
+      <c r="J3" s="6"/>
+      <c r="M3" t="s">
         <v>44</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:16">
+      <c r="B4" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="43.2">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:16" ht="45">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="H5" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="57.6">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="1:16" ht="60">
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="H6" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="O6" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="1:16">
+      <c r="C7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="J7" s="10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="28.8">
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="1:16" ht="30">
+      <c r="C8" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>53</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>39</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="J8" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
-      <c r="C9" s="9" t="s">
+    <row r="9" spans="1:16">
+      <c r="D9" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>54</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>64</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="J9" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
-      <c r="E10" t="s">
+    <row r="10" spans="1:16">
+      <c r="F10" t="s">
         <v>56</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="J10" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
-      <c r="E11" t="s">
+    <row r="11" spans="1:16">
+      <c r="F11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
-      <c r="I12" s="11" t="s">
+    <row r="12" spans="1:16">
+      <c r="J12" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
-      <c r="E13" s="10" t="s">
+    <row r="13" spans="1:16">
+      <c r="F13" s="10" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP : Add Asus AutoStart Intent
</commit_message>
<xml_diff>
--- a/table_device_package.xlsx
+++ b/table_device_package.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>DEVICES</t>
   </si>
@@ -586,6 +586,9 @@
       </rPr>
       <t>+new ComponentName("com.oneplus.security", "com.oneplus.security.chainlaunch.view" + ".ChainLaunchAppListActivity"</t>
     </r>
+  </si>
+  <si>
+    <t>new ComponentName("com.asus.powersaver", "com.asus.powersaver.PowerSaverSettings")</t>
   </si>
 </sst>
 </file>
@@ -1072,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1290,6 +1293,9 @@
       <c r="G7" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="H7" t="s">
+        <v>79</v>
+      </c>
       <c r="I7" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
ADD changelog, Asus compatibility and improve README
</commit_message>
<xml_diff>
--- a/table_device_package.xlsx
+++ b/table_device_package.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T0173711\AndroidStudioProjects\AppKillerManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\StudioProjects\AppKillerManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -414,11 +414,100 @@
     <t>com.meizu.safe.powerui.PowerAppPermissionActivity == com.meizu.power.PowerAppKilledNotification</t>
   </si>
   <si>
+    <t>ONEPLUS</t>
+  </si>
+  <si>
+    <r>
+      <t>"oppo com.coloros.oppoguardelf"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008800"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>"com.coloros.powermanager.fuelgaue.PowerUsageModelActivity</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">autostart : new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>ComponentName(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"com.oneplus.security"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">"com.oneplus.security.chainlaunch.view" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>+new ComponentName("com.oneplus.security", "com.oneplus.security.chainlaunch.view" + ".ChainLaunchAppListActivity"</t>
+    </r>
+  </si>
+  <si>
+    <t>new ComponentName("com.asus.powersaver", "com.asus.powersaver.PowerSaverSettings")</t>
+  </si>
+  <si>
+    <t>HTC</t>
+  </si>
+  <si>
+    <t>Intent().setComponent(ComponentName("com.htc.pitroad", "com.htc.pitroad.landingpage.activity.LandingPageActivity"))</t>
+  </si>
+  <si>
+    <t>background battery</t>
+  </si>
+  <si>
     <r>
       <t>new</t>
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="8"/>
         <color rgb="FF303336"/>
         <rFont val="Inherit"/>
@@ -427,6 +516,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="8"/>
         <color rgb="FF2B91AF"/>
         <rFont val="Inherit"/>
@@ -435,6 +525,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="8"/>
         <color rgb="FF303336"/>
         <rFont val="Inherit"/>
@@ -443,6 +534,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="8"/>
         <color rgb="FF7D2727"/>
         <rFont val="Inherit"/>
@@ -451,6 +543,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="8"/>
         <color rgb="FF303336"/>
         <rFont val="Inherit"/>
@@ -459,6 +552,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="8"/>
         <color rgb="FF7D2727"/>
         <rFont val="Inherit"/>
@@ -467,6 +561,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="8"/>
         <color rgb="FF303336"/>
         <rFont val="Inherit"/>
@@ -480,6 +575,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="8"/>
         <color rgb="FF2B91AF"/>
         <rFont val="Inherit"/>
@@ -488,6 +584,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="8"/>
         <color rgb="FF303336"/>
         <rFont val="Inherit"/>
@@ -496,6 +593,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="8"/>
         <color rgb="FF7D2727"/>
         <rFont val="Inherit"/>
@@ -504,107 +602,20 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="8"/>
         <color rgb="FF303336"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>))</t>
     </r>
-  </si>
-  <si>
-    <t>ONEPLUS</t>
-  </si>
-  <si>
-    <r>
-      <t>"oppo com.coloros.oppoguardelf"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF333333"/>
-        <rFont val="Source Code Pro"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF008800"/>
-        <rFont val="Source Code Pro"/>
-        <family val="3"/>
-      </rPr>
-      <t>"com.coloros.powermanager.fuelgaue.PowerUsageModelActivity</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">autostart : new </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>ComponentName(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>"com.oneplus.security"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">"com.oneplus.security.chainlaunch.view" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFA9B7C6"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>+new ComponentName("com.oneplus.security", "com.oneplus.security.chainlaunch.view" + ".ChainLaunchAppListActivity"</t>
-    </r>
-  </si>
-  <si>
-    <t>new ComponentName("com.asus.powersaver", "com.asus.powersaver.PowerSaverSettings")</t>
-  </si>
-  <si>
-    <t>HTC</t>
-  </si>
-  <si>
-    <t>Intent().setComponent(ComponentName("com.htc.pitroad", "com.htc.pitroad.landingpage.activity.LandingPageActivity"))</t>
-  </si>
-  <si>
-    <t>background battery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -692,26 +703,6 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF101094"/>
-      <name val="Inherit"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF303336"/>
-      <name val="Inherit"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF2B91AF"/>
-      <name val="Inherit"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF7D2727"/>
-      <name val="Inherit"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Source Code Pro"/>
@@ -722,6 +713,38 @@
       <color rgb="FF008800"/>
       <name val="Source Code Pro"/>
       <family val="3"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="8"/>
+      <color rgb="FF101094"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="8"/>
+      <color rgb="FF303336"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="8"/>
+      <color rgb="FF2B91AF"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="8"/>
+      <color rgb="FF7D2727"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -756,7 +779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -787,21 +810,22 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="6"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1084,27 +1108,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="115.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="94.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="149.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.85546875" customWidth="1"/>
-    <col min="8" max="8" width="79.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="112.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="91.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="75.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="115.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="94.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="149.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.88671875" customWidth="1"/>
+    <col min="8" max="8" width="79.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="112.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="72.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="91.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="75.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -1112,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1139,7 +1163,7 @@
         <v>33</v>
       </c>
       <c r="Q1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1186,9 +1210,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="105">
-      <c r="B3" s="15" t="s">
-        <v>78</v>
+    <row r="3" spans="1:17" ht="100.8">
+      <c r="B3" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -1222,11 +1246,11 @@
         <v>62</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="B4" s="14"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1249,10 +1273,10 @@
         <v>48</v>
       </c>
       <c r="Q4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="45">
+    <row r="5" spans="1:17" ht="43.2">
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1262,8 +1286,8 @@
       <c r="G5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>74</v>
+      <c r="H5" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="I5" t="s">
         <v>36</v>
@@ -1272,7 +1296,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="60">
+    <row r="6" spans="1:17" ht="57.6">
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1285,8 +1309,8 @@
       <c r="G6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="13" t="s">
-        <v>75</v>
+      <c r="H6" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="I6" t="s">
         <v>37</v>
@@ -1311,8 +1335,8 @@
       <c r="G7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H7" t="s">
-        <v>79</v>
+      <c r="H7" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="I7" t="s">
         <v>51</v>
@@ -1321,7 +1345,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="30">
+    <row r="8" spans="1:17" ht="28.8">
       <c r="C8" s="5" t="s">
         <v>63</v>
       </c>
@@ -1345,8 +1369,8 @@
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="C9" s="16" t="s">
-        <v>77</v>
+      <c r="C9" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
Add ZTE compatiblity, fix exemple, improve Dialog UI, Add screenshot for Asus
</commit_message>
<xml_diff>
--- a/table_device_package.xlsx
+++ b/table_device_package.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T0173711\AndroidStudioProjects\AppKillerManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\StudioProjects\AppKillerManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1133,26 +1133,26 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="115.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="94.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="149.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.85546875" customWidth="1"/>
-    <col min="8" max="8" width="79.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="112.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="91.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="75.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="115.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="94.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="149.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.88671875" customWidth="1"/>
+    <col min="8" max="8" width="79.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="112.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="72.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="91.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="75.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -1234,7 +1234,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="105">
+    <row r="3" spans="1:17" ht="100.8">
       <c r="B3" s="13" t="s">
         <v>75</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="45">
+    <row r="5" spans="1:17" ht="43.2">
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="60">
+    <row r="6" spans="1:17" ht="57.6">
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="30">
+    <row r="8" spans="1:17" ht="28.8">
       <c r="C8" s="5" t="s">
         <v>63</v>
       </c>

</xml_diff>